<commit_message>
Added templates to several model3d polygon data classes so that vertex data with tangent vectors is only used for bump mapped materials, which reduces memory in the case where bump maps are not used. -FG
</commit_message>
<xml_diff>
--- a/scene_stats.xlsx
+++ b/scene_stats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>Scene</t>
   </si>
@@ -67,6 +67,15 @@
   </si>
   <si>
     <t>Conference</t>
+  </si>
+  <si>
+    <t>Has Normals</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -408,280 +417,437 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="1" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="5.140625" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" customWidth="1"/>
+    <col min="14" max="14" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="K1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="2">
         <v>39742</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D2" s="2">
         <v>41438</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>0.8</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>1.4</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>174</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>155</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>165</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="K2">
+        <v>0.8</v>
+      </c>
+      <c r="L2">
+        <v>174</v>
+      </c>
+      <c r="M2">
+        <v>155</v>
+      </c>
+      <c r="N2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2">
         <v>153635</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3" s="2">
         <v>144101</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>4</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>7.8</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>521</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>492</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>115</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="K3">
+        <v>8.1</v>
+      </c>
+      <c r="L3">
+        <v>521</v>
+      </c>
+      <c r="M3">
+        <v>483</v>
+      </c>
+      <c r="N3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="2">
         <v>40981</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4" s="2">
         <v>75165</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>1.4</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>118</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>97</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>400</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="K4">
+        <v>1.4</v>
+      </c>
+      <c r="L4">
+        <v>114</v>
+      </c>
+      <c r="M4">
+        <v>96</v>
+      </c>
+      <c r="N4">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2">
         <v>194399</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D5" s="2">
         <v>330837</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>4.7</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>8.1</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>407</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>268</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>340</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="K5">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="L5">
+        <v>391</v>
+      </c>
+      <c r="M5">
+        <v>251</v>
+      </c>
+      <c r="N5">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2">
         <v>435545</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D6" s="2">
         <v>871198</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>13.1</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>14.3</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>242</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>166</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>210</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="K6">
+        <v>15.6</v>
+      </c>
+      <c r="L6">
+        <v>242</v>
+      </c>
+      <c r="M6">
+        <v>114</v>
+      </c>
+      <c r="N6">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="2">
         <v>543524</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D7" s="2">
         <v>1087304</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>16.5</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>18</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>276</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>188</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>185</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="K7">
+        <v>18.8</v>
+      </c>
+      <c r="L7">
+        <v>275</v>
+      </c>
+      <c r="M7">
+        <v>120</v>
+      </c>
+      <c r="N7">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="2">
         <v>1470000</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D8" s="2">
         <v>2850000</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>44</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>48</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>571</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>353</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>62</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="K8">
+        <v>49</v>
+      </c>
+      <c r="L8">
+        <v>570</v>
+      </c>
+      <c r="M8">
+        <v>167</v>
+      </c>
+      <c r="N8">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="2">
         <v>4488339</v>
       </c>
-      <c r="C9" s="2">
+      <c r="D9" s="2">
         <v>6481796</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>96</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>107</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>1243</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>855</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="K9">
+        <v>111</v>
+      </c>
+      <c r="L9">
+        <v>1326</v>
+      </c>
+      <c r="M9">
+        <v>679</v>
+      </c>
+      <c r="N9">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="2">
         <v>5489773</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D10" s="2">
         <v>2169124</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>127</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>131</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>709</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>304</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>86</v>
+      </c>
+      <c r="K10">
+        <v>137</v>
+      </c>
+      <c r="L10">
+        <v>740</v>
+      </c>
+      <c r="M10">
+        <v>295</v>
+      </c>
+      <c r="N10">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed poly_data_block to store vertex data by index instead of value, added remove_excess_cap_calls, and made some other changes that decrease peak memory during model3d load. -FG
</commit_message>
<xml_diff>
--- a/scene_stats.xlsx
+++ b/scene_stats.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="28755" windowHeight="14370"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="16635" windowHeight="7140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -420,7 +420,7 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -636,7 +636,7 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="L5">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="M5">
         <v>251</v>
@@ -677,7 +677,7 @@
         <v>15.6</v>
       </c>
       <c r="L6">
-        <v>242</v>
+        <v>164</v>
       </c>
       <c r="M6">
         <v>114</v>
@@ -718,7 +718,7 @@
         <v>18.8</v>
       </c>
       <c r="L7">
-        <v>275</v>
+        <v>181</v>
       </c>
       <c r="M7">
         <v>120</v>
@@ -759,7 +759,7 @@
         <v>49</v>
       </c>
       <c r="L8">
-        <v>570</v>
+        <v>327</v>
       </c>
       <c r="M8">
         <v>167</v>
@@ -800,7 +800,7 @@
         <v>111</v>
       </c>
       <c r="L9">
-        <v>1326</v>
+        <v>888</v>
       </c>
       <c r="M9">
         <v>679</v>
@@ -841,7 +841,7 @@
         <v>137</v>
       </c>
       <c r="L10">
-        <v>740</v>
+        <v>566</v>
       </c>
       <c r="M10">
         <v>295</v>

</xml_diff>

<commit_message>
Increased MAX_VMAP_SIZE from 64K to 256K, which seems to work a little better on the soda scene. -FG
</commit_message>
<xml_diff>
--- a/scene_stats.xlsx
+++ b/scene_stats.xlsx
@@ -420,7 +420,7 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -841,13 +841,13 @@
         <v>137</v>
       </c>
       <c r="L10">
-        <v>566</v>
+        <v>525</v>
       </c>
       <c r="M10">
-        <v>295</v>
+        <v>254</v>
       </c>
       <c r="N10">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>